<commit_message>
Fixed ransacker search for enum distribution_on in CD
</commit_message>
<xml_diff>
--- a/public/sample_uploads/kpi_extraction/MIS Sample4.xlsx
+++ b/public/sample_uploads/kpi_extraction/MIS Sample4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\kpi_extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0559029-1472-4CF2-9785-CD0A6EF34B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA70E317-99FC-4EA6-A67A-CCA97360BBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{D76C8113-FF3C-43E7-B858-2AB9C8FB14CC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="1" xr2:uid="{D76C8113-FF3C-43E7-B858-2AB9C8FB14CC}"/>
   </bookViews>
   <sheets>
     <sheet name="A. Quarterly data" sheetId="94" r:id="rId1"/>
@@ -260,16 +260,16 @@
     <t>5) There could be some totalling anomalies in the numbers displayed above due to the impact of rounding off.</t>
   </si>
   <si>
-    <t>Food Delivery 'GOV</t>
-  </si>
-  <si>
     <t>Adjusted EBITDA Food dlivery</t>
   </si>
   <si>
-    <t xml:space="preserve"> Hyperpure Revenue</t>
+    <t>Hyperpure Adjusted EBITDA</t>
   </si>
   <si>
-    <t>Hyperpure Adjusted EBITDA</t>
+    <t>Food Delivery GOV</t>
+  </si>
+  <si>
+    <t>Hyperpure Revenue</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1015,7 @@
   </sheetPr>
   <dimension ref="A1:XFC112"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -51099,8 +51099,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -51159,7 +51159,7 @@
     <row r="3" spans="1:12" ht="18.399999999999999" x14ac:dyDescent="0.65">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C3" s="18">
         <v>54.07</v>
@@ -51287,7 +51287,7 @@
     <row r="7" spans="1:12" ht="18.399999999999999" x14ac:dyDescent="0.65">
       <c r="A7" s="1"/>
       <c r="B7" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="18">
         <v>-2.29</v>
@@ -51597,7 +51597,7 @@
     <row r="21" spans="1:12" ht="18.399999999999999" x14ac:dyDescent="0.65">
       <c r="A21" s="1"/>
       <c r="B21" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C21" s="18">
         <v>1.1200000000000001</v>
@@ -51661,7 +51661,7 @@
     <row r="23" spans="1:12" ht="18.399999999999999" x14ac:dyDescent="0.65">
       <c r="A23" s="1"/>
       <c r="B23" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C23" s="18">
         <v>-0.3</v>

</xml_diff>